<commit_message>
further dev on hands on 3
</commit_message>
<xml_diff>
--- a/Uebung_3/doc/simulink-luna-landing-results.xlsx
+++ b/Uebung_3/doc/simulink-luna-landing-results.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Start Thrust 1</t>
   </si>
@@ -64,13 +64,28 @@
   </si>
   <si>
     <t>euler</t>
+  </si>
+  <si>
+    <t>h(t) div</t>
+  </si>
+  <si>
+    <t>v(t) div</t>
+  </si>
+  <si>
+    <t>Aufgabe 1 a.</t>
+  </si>
+  <si>
+    <t>Aufgabe 1 b. 2</t>
+  </si>
+  <si>
+    <t>Aufgabe 1 b. 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +100,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -94,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -456,11 +479,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -508,11 +604,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -822,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A17" sqref="A17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,170 +994,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B3" s="12">
         <v>29</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C3" s="13">
         <v>53.2</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D3" s="12">
         <v>14.8</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E3" s="13">
         <v>38</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F3" s="22">
         <v>-8.8015623023849996E-3</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G3" s="19">
         <v>-7.1718099504634303</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B4" s="14">
         <v>13</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C4" s="15">
         <v>55</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D4" s="14">
         <v>30.8</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E4" s="15">
         <v>44</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F4" s="23">
         <v>-2.5865029793547999E-2</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G4" s="20">
         <v>-8.7178649701106696</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B5" s="16">
         <v>22</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C5" s="18">
         <v>48.8</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D5" s="16">
         <v>19.8</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E5" s="18">
         <v>40.799999999999997</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F5" s="24">
         <v>1.799327586801E-3</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G5" s="21">
         <v>-1.4410215049190001</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="27"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2">
-        <v>48.8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>19.8</v>
-      </c>
-      <c r="E6" s="3">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.799327586801E-3</v>
-      </c>
-      <c r="H6" s="15">
-        <v>-1.4410215049190001</v>
-      </c>
+      <c r="A6" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1021,42 +1129,67 @@
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1">
-        <v>-5.784244328044E-3</v>
-      </c>
-      <c r="H7" s="15">
-        <v>-0.31360982553713002</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="17">
-        <v>-1.92230842885561</v>
-      </c>
-      <c r="H8" s="18">
-        <v>-9.5930923294489805</v>
+      <c r="A8" s="30">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <v>48.8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19.8</v>
+      </c>
+      <c r="E8" s="3">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.799327586801E-3</v>
+      </c>
+      <c r="H8" s="15">
+        <v>-1.4410215049190001</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1070,30 +1203,20 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>5</v>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-5.784244328044E-3</v>
+      </c>
+      <c r="H9" s="15">
+        <v>-0.31360982553713002</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1108,75 +1231,329 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+      <c r="F10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="17">
+        <v>-1.92230842885561</v>
+      </c>
+      <c r="H10" s="18">
+        <v>-9.5930923294489805</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2">
+      <c r="F12" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>1</v>
+      </c>
+      <c r="B13" s="2">
         <v>22</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C13" s="2">
         <v>48.8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D13" s="2">
         <v>19.8</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E13" s="3">
         <v>40.799999999999997</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G13" s="1">
         <v>1.799327586801E-3</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H13" s="15">
         <v>-1.4410215049190001</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="14" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G14" s="1">
         <v>-2.1843000000000001E-3</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H14" s="15">
         <v>-1.6194999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="14" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G15" s="1">
         <v>-2.1854000000000001E-3</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H15" s="15">
         <v>-1.5762</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="16" t="s">
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G16" s="17">
         <v>-2.1856000000000002E-3</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H16" s="18">
         <v>-0.42630000000000001</v>
       </c>
     </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="12">
+        <v>29</v>
+      </c>
+      <c r="C19" s="13">
+        <v>53.2</v>
+      </c>
+      <c r="D19" s="12">
+        <v>14.8</v>
+      </c>
+      <c r="E19" s="13">
+        <v>38</v>
+      </c>
+      <c r="F19" s="22">
+        <v>-6.8529809796201005E-2</v>
+      </c>
+      <c r="G19" s="19">
+        <v>-6.90871822135247</v>
+      </c>
+      <c r="H19" s="22">
+        <v>-8.8015623023849996E-3</v>
+      </c>
+      <c r="I19" s="31">
+        <v>-7.1718099504634303</v>
+      </c>
+      <c r="J19" s="34">
+        <f>H19-F19</f>
+        <v>5.9728247493816007E-2</v>
+      </c>
+      <c r="K19" s="35">
+        <f>I19-G19</f>
+        <v>-0.26309172911096024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>2</v>
+      </c>
+      <c r="B20" s="14">
+        <v>13</v>
+      </c>
+      <c r="C20" s="15">
+        <v>55</v>
+      </c>
+      <c r="D20" s="14">
+        <v>30.8</v>
+      </c>
+      <c r="E20" s="15">
+        <v>44</v>
+      </c>
+      <c r="F20" s="23">
+        <v>-3.2871105771640999E-2</v>
+      </c>
+      <c r="G20" s="20">
+        <v>-8.0878671799161204</v>
+      </c>
+      <c r="H20" s="23">
+        <v>-2.5865029793547999E-2</v>
+      </c>
+      <c r="I20" s="32">
+        <v>-8.7178649701106696</v>
+      </c>
+      <c r="J20" s="36">
+        <f t="shared" ref="J20:J21" si="0">H20-F20</f>
+        <v>7.0060759780929995E-3</v>
+      </c>
+      <c r="K20" s="37">
+        <f t="shared" ref="K20:K21" si="1">I20-G20</f>
+        <v>-0.62999779019454927</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>3</v>
+      </c>
+      <c r="B21" s="16">
+        <v>22</v>
+      </c>
+      <c r="C21" s="18">
+        <v>48.8</v>
+      </c>
+      <c r="D21" s="16">
+        <v>19.8</v>
+      </c>
+      <c r="E21" s="18">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F21" s="24">
+        <v>-8.80521096965E-3</v>
+      </c>
+      <c r="G21" s="21">
+        <v>-3.4122670705121498</v>
+      </c>
+      <c r="H21" s="24">
+        <v>1.799327586801E-3</v>
+      </c>
+      <c r="I21" s="33">
+        <v>-1.4410215049190001</v>
+      </c>
+      <c r="J21" s="38">
+        <f t="shared" si="0"/>
+        <v>1.0604538556451E-2</v>
+      </c>
+      <c r="K21" s="39">
+        <f t="shared" si="1"/>
+        <v>1.9712455655931498</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A17:G17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J19:K21">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>